<commit_message>
[U] update the BOM
</commit_message>
<xml_diff>
--- a/circuit/BOM.xlsx
+++ b/circuit/BOM.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$L$18</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +210,126 @@
   </si>
   <si>
     <t>1.516m</t>
+  </si>
+  <si>
+    <t>Val.@footprint</t>
+  </si>
+  <si>
+    <t>100u@0805</t>
+  </si>
+  <si>
+    <t>110k@0805</t>
+  </si>
+  <si>
+    <t>11k@0805</t>
+  </si>
+  <si>
+    <t>100n@0805</t>
+  </si>
+  <si>
+    <t>150k@0805</t>
+  </si>
+  <si>
+    <t>33k@0805</t>
+  </si>
+  <si>
+    <t>56k@0805</t>
+  </si>
+  <si>
+    <t>10k@0805</t>
+  </si>
+  <si>
+    <t>1.5M@0805</t>
+  </si>
+  <si>
+    <t>47p@0805</t>
+  </si>
+  <si>
+    <t>4.7p@0805</t>
+  </si>
+  <si>
+    <t>3.3n@0805</t>
+  </si>
+  <si>
+    <t>4.7n@0805</t>
+  </si>
+  <si>
+    <t>4.7u@0805</t>
+  </si>
+  <si>
+    <t>(1n,2.2n,3.3n)@0805</t>
+  </si>
+  <si>
+    <t>10V470u@6*12</t>
+  </si>
+  <si>
+    <t>ss24@sma</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>1k@0805</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>1n@0805</t>
+  </si>
+  <si>
+    <t>2.2@0805</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>SS24</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>C_e</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>电子元件配单 订单 电子元器件 IC芯片二三极管电容电阻 差价补拍</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>74HC244D@SOP20</t>
+  </si>
+  <si>
+    <t>74HC244</t>
+  </si>
+  <si>
+    <t>非Risym</t>
+  </si>
+  <si>
+    <t>BTN7971B</t>
+  </si>
+  <si>
+    <t>（淘宝）</t>
+  </si>
+  <si>
+    <t>TPS54160</t>
+  </si>
+  <si>
+    <t>（学校）</t>
   </si>
 </sst>
 </file>
@@ -238,7 +361,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -246,18 +369,181 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,374 +826,884 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="9" max="9" width="20.6328125" customWidth="1"/>
+    <col min="11" max="11" width="20.6328125" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4"/>
+      <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="I2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="4">
+        <v>3</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="I3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="4">
+        <v>3</v>
+      </c>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="I4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="I5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="I6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="I7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="I8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="I9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="I10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="I11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="I12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="4">
+        <v>8</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2</v>
+      </c>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="I14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2</v>
+      </c>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="I15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2</v>
+      </c>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="I16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2</v>
+      </c>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E13:G13"/>
+  <sortState ref="J2:L19">
+    <sortCondition ref="J2:J19"/>
+    <sortCondition descending="1" ref="L2:L19"/>
+  </sortState>
+  <mergeCells count="11">
+    <mergeCell ref="M2:M8"/>
+    <mergeCell ref="M12:M18"/>
     <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F17:I18"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1"/>
+    <hyperlink ref="F13" r:id="rId1"/>
     <hyperlink ref="B13" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="I12" r:id="rId5"/>
+    <hyperlink ref="I2" r:id="rId6"/>
+    <hyperlink ref="E3" r:id="rId7"/>
+    <hyperlink ref="I3" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="I4" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
+    <hyperlink ref="I6" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="I14" r:id="rId14"/>
+    <hyperlink ref="E15" r:id="rId15"/>
+    <hyperlink ref="I15" r:id="rId16"/>
+    <hyperlink ref="E9" r:id="rId17"/>
+    <hyperlink ref="I9" r:id="rId18"/>
+    <hyperlink ref="E5" r:id="rId19"/>
+    <hyperlink ref="I5" r:id="rId20"/>
+    <hyperlink ref="E7" r:id="rId21"/>
+    <hyperlink ref="I7" r:id="rId22"/>
+    <hyperlink ref="E11" r:id="rId23"/>
+    <hyperlink ref="I11" r:id="rId24"/>
+    <hyperlink ref="E10" r:id="rId25"/>
+    <hyperlink ref="I10" r:id="rId26"/>
+    <hyperlink ref="E16" r:id="rId27"/>
+    <hyperlink ref="I16" r:id="rId28"/>
+    <hyperlink ref="E13" r:id="rId29"/>
+    <hyperlink ref="I13" r:id="rId30"/>
+    <hyperlink ref="K1" r:id="rId31"/>
+    <hyperlink ref="K13" r:id="rId32"/>
+    <hyperlink ref="K14" r:id="rId33"/>
+    <hyperlink ref="K5" r:id="rId34"/>
+    <hyperlink ref="K6" r:id="rId35"/>
+    <hyperlink ref="K15" r:id="rId36"/>
+    <hyperlink ref="K2" r:id="rId37"/>
+    <hyperlink ref="K3" r:id="rId38"/>
+    <hyperlink ref="K7" r:id="rId39"/>
+    <hyperlink ref="K8" r:id="rId40"/>
+    <hyperlink ref="K19" r:id="rId41"/>
+    <hyperlink ref="K4" r:id="rId42"/>
+    <hyperlink ref="K11" r:id="rId43"/>
+    <hyperlink ref="K10" r:id="rId44"/>
+    <hyperlink ref="K17" r:id="rId45"/>
+    <hyperlink ref="K18" r:id="rId46"/>
+    <hyperlink ref="K16" r:id="rId47"/>
+    <hyperlink ref="K12" r:id="rId48"/>
+    <hyperlink ref="M10" r:id="rId49"/>
+    <hyperlink ref="M2:M4" r:id="rId50" display="C"/>
+    <hyperlink ref="K9" r:id="rId51"/>
+    <hyperlink ref="M9" r:id="rId52"/>
+    <hyperlink ref="M12:M18" r:id="rId53" display="R"/>
+    <hyperlink ref="M19" r:id="rId54"/>
+    <hyperlink ref="M11" r:id="rId55"/>
+    <hyperlink ref="K20" r:id="rId56"/>
+    <hyperlink ref="M20" r:id="rId57"/>
+    <hyperlink ref="A18" r:id="rId58"/>
+    <hyperlink ref="A19:B19" r:id="rId59" display="TPS54160"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>